<commit_message>
Update Progress Data Preprocessing
</commit_message>
<xml_diff>
--- a/Datasets_Politik_v2_CakNun.xlsx
+++ b/Datasets_Politik_v2_CakNun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kuliah\Semester 8\Skripsi\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAFFB7B-324C-4A24-AA0A-885293217C7A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909C369B-990D-4CDF-9CD3-110A561B1534}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5729,9 +5729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D889"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>